<commit_message>
implemented random forest, odds and fixed regression
</commit_message>
<xml_diff>
--- a/results/regression_results.xlsx
+++ b/results/regression_results.xlsx
@@ -38,12 +38,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
+        <fgColor rgb="00008000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00008000"/>
+        <fgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -489,7 +489,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -499,7 +499,7 @@
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>V</t>
         </is>
       </c>
     </row>
@@ -527,7 +527,7 @@
           <t>2-2</t>
         </is>
       </c>
-      <c r="F3" s="2" t="inlineStr">
+      <c r="F3" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -557,7 +557,7 @@
           <t>0-1</t>
         </is>
       </c>
-      <c r="F4" s="2" t="inlineStr">
+      <c r="F4" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -587,7 +587,7 @@
           <t>1-1</t>
         </is>
       </c>
-      <c r="F5" s="3" t="inlineStr">
+      <c r="F5" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -609,7 +609,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -617,7 +617,7 @@
           <t>3-2</t>
         </is>
       </c>
-      <c r="F6" s="3" t="inlineStr">
+      <c r="F6" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -647,7 +647,7 @@
           <t>0-1</t>
         </is>
       </c>
-      <c r="F7" s="2" t="inlineStr">
+      <c r="F7" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -669,7 +669,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -677,7 +677,7 @@
           <t>1-2</t>
         </is>
       </c>
-      <c r="F8" s="2" t="inlineStr">
+      <c r="F8" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -699,7 +699,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1-1</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -709,7 +709,7 @@
       </c>
       <c r="F9" s="2" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>V</t>
         </is>
       </c>
     </row>
@@ -737,7 +737,7 @@
           <t>1-3</t>
         </is>
       </c>
-      <c r="F10" s="2" t="inlineStr">
+      <c r="F10" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -759,7 +759,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>0-2</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -767,7 +767,7 @@
           <t>2-2</t>
         </is>
       </c>
-      <c r="F11" s="2" t="inlineStr">
+      <c r="F11" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -789,7 +789,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2-0</t>
+          <t>3-1</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -797,7 +797,7 @@
           <t>1-0</t>
         </is>
       </c>
-      <c r="F12" s="3" t="inlineStr">
+      <c r="F12" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -819,7 +819,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -829,7 +829,7 @@
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>X</t>
         </is>
       </c>
     </row>
@@ -857,7 +857,7 @@
           <t>1-2</t>
         </is>
       </c>
-      <c r="F14" s="2" t="inlineStr">
+      <c r="F14" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -879,7 +879,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -887,7 +887,7 @@
           <t>2-2</t>
         </is>
       </c>
-      <c r="F15" s="2" t="inlineStr">
+      <c r="F15" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -909,7 +909,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -917,7 +917,7 @@
           <t>1-4</t>
         </is>
       </c>
-      <c r="F16" s="3" t="inlineStr">
+      <c r="F16" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -939,7 +939,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>X</t>
         </is>
       </c>
     </row>
@@ -969,7 +969,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -977,7 +977,7 @@
           <t>2-0</t>
         </is>
       </c>
-      <c r="F18" s="2" t="inlineStr">
+      <c r="F18" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -999,7 +999,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1007,7 +1007,7 @@
           <t>2-1</t>
         </is>
       </c>
-      <c r="F19" s="3" t="inlineStr">
+      <c r="F19" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -1029,15 +1029,15 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
+          <t>2-1</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
           <t>2-0</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>2-0</t>
-        </is>
-      </c>
-      <c r="F20" s="3" t="inlineStr">
+      <c r="F20" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1-1</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1069,7 +1069,7 @@
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>X</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1097,7 +1097,7 @@
           <t>0-4</t>
         </is>
       </c>
-      <c r="F22" s="3" t="inlineStr">
+      <c r="F22" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -1127,7 +1127,7 @@
           <t>3-3</t>
         </is>
       </c>
-      <c r="F23" s="3" t="inlineStr">
+      <c r="F23" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1159,7 +1159,7 @@
       </c>
       <c r="F24" s="3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>X</t>
         </is>
       </c>
     </row>
@@ -1179,17 +1179,17 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
+          <t>1-1</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
           <t>1-0</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>1-0</t>
-        </is>
-      </c>
       <c r="F25" s="3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>X</t>
         </is>
       </c>
     </row>
@@ -1209,15 +1209,15 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
+          <t>1-1</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
           <t>0-0</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>0-0</t>
-        </is>
-      </c>
-      <c r="F26" s="3" t="inlineStr">
+      <c r="F26" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -1239,7 +1239,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1247,7 +1247,7 @@
           <t>3-2</t>
         </is>
       </c>
-      <c r="F27" s="3" t="inlineStr">
+      <c r="F27" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -1277,7 +1277,7 @@
           <t>0-0</t>
         </is>
       </c>
-      <c r="F28" s="3" t="inlineStr">
+      <c r="F28" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -1307,7 +1307,7 @@
           <t>0-0</t>
         </is>
       </c>
-      <c r="F29" s="3" t="inlineStr">
+      <c r="F29" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2-0</t>
+          <t>3-1</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1337,7 +1337,7 @@
           <t>0-2</t>
         </is>
       </c>
-      <c r="F30" s="2" t="inlineStr">
+      <c r="F30" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1359,7 +1359,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1367,7 +1367,7 @@
           <t>1-3</t>
         </is>
       </c>
-      <c r="F31" s="3" t="inlineStr">
+      <c r="F31" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -1397,7 +1397,7 @@
           <t>1-1</t>
         </is>
       </c>
-      <c r="F32" s="3" t="inlineStr">
+      <c r="F32" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1427,7 +1427,7 @@
           <t>1-2</t>
         </is>
       </c>
-      <c r="F33" s="3" t="inlineStr">
+      <c r="F33" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -1457,7 +1457,7 @@
           <t>0-0</t>
         </is>
       </c>
-      <c r="F34" s="3" t="inlineStr">
+      <c r="F34" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -1479,7 +1479,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1489,7 +1489,7 @@
       </c>
       <c r="F35" s="3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>X</t>
         </is>
       </c>
     </row>
@@ -1517,7 +1517,7 @@
           <t>1-0</t>
         </is>
       </c>
-      <c r="F36" s="3" t="inlineStr">
+      <c r="F36" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -1539,7 +1539,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1547,7 +1547,7 @@
           <t>3-2</t>
         </is>
       </c>
-      <c r="F37" s="3" t="inlineStr">
+      <c r="F37" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1579,7 +1579,7 @@
       </c>
       <c r="F38" s="3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>X</t>
         </is>
       </c>
     </row>
@@ -1599,7 +1599,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>1-1</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1607,7 +1607,7 @@
           <t>2-0</t>
         </is>
       </c>
-      <c r="F39" s="2" t="inlineStr">
+      <c r="F39" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1629,15 +1629,15 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
+          <t>1-3</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
           <t>0-2</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>0-2</t>
-        </is>
-      </c>
-      <c r="F40" s="3" t="inlineStr">
+      <c r="F40" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1667,7 +1667,7 @@
           <t>1-2</t>
         </is>
       </c>
-      <c r="F41" s="3" t="inlineStr">
+      <c r="F41" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -1697,7 +1697,7 @@
           <t>1-1</t>
         </is>
       </c>
-      <c r="F42" s="3" t="inlineStr">
+      <c r="F42" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -1719,7 +1719,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1727,7 +1727,7 @@
           <t>0-3</t>
         </is>
       </c>
-      <c r="F43" s="3" t="inlineStr">
+      <c r="F43" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -1749,7 +1749,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1759,7 +1759,7 @@
       </c>
       <c r="F44" s="3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>X</t>
         </is>
       </c>
     </row>
@@ -1779,7 +1779,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0-0</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -1789,7 +1789,7 @@
       </c>
       <c r="F45" s="2" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>V</t>
         </is>
       </c>
     </row>
@@ -1817,7 +1817,7 @@
           <t>1-0</t>
         </is>
       </c>
-      <c r="F46" s="3" t="inlineStr">
+      <c r="F46" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>0-2</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1847,7 +1847,7 @@
           <t>0-3</t>
         </is>
       </c>
-      <c r="F47" s="3" t="inlineStr">
+      <c r="F47" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1877,7 +1877,7 @@
           <t>0-3</t>
         </is>
       </c>
-      <c r="F48" s="3" t="inlineStr">
+      <c r="F48" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -1899,7 +1899,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>1-1</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -1907,7 +1907,7 @@
           <t>2-3</t>
         </is>
       </c>
-      <c r="F49" s="2" t="inlineStr">
+      <c r="F49" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1929,7 +1929,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -1937,7 +1937,7 @@
           <t>2-3</t>
         </is>
       </c>
-      <c r="F50" s="3" t="inlineStr">
+      <c r="F50" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -1959,7 +1959,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -1967,7 +1967,7 @@
           <t>0-1</t>
         </is>
       </c>
-      <c r="F51" s="2" t="inlineStr">
+      <c r="F51" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1989,17 +1989,17 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
+          <t>1-1</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
           <t>1-0</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>1-0</t>
-        </is>
-      </c>
       <c r="F52" s="3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>X</t>
         </is>
       </c>
     </row>
@@ -2019,7 +2019,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -2029,7 +2029,7 @@
       </c>
       <c r="F53" s="2" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>V</t>
         </is>
       </c>
     </row>
@@ -2057,7 +2057,7 @@
           <t>1-3</t>
         </is>
       </c>
-      <c r="F54" s="2" t="inlineStr">
+      <c r="F54" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -2079,7 +2079,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2-0</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -2087,7 +2087,7 @@
           <t>2-2</t>
         </is>
       </c>
-      <c r="F55" s="2" t="inlineStr">
+      <c r="F55" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -2109,7 +2109,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2-0</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -2117,7 +2117,7 @@
           <t>0-3</t>
         </is>
       </c>
-      <c r="F56" s="2" t="inlineStr">
+      <c r="F56" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -2147,7 +2147,7 @@
           <t>1-1</t>
         </is>
       </c>
-      <c r="F57" s="3" t="inlineStr">
+      <c r="F57" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -2177,7 +2177,7 @@
           <t>3-2</t>
         </is>
       </c>
-      <c r="F58" s="3" t="inlineStr">
+      <c r="F58" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -2199,7 +2199,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>0-2</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2207,7 +2207,7 @@
           <t>1-2</t>
         </is>
       </c>
-      <c r="F59" s="3" t="inlineStr">
+      <c r="F59" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -2237,7 +2237,7 @@
           <t>1-0</t>
         </is>
       </c>
-      <c r="F60" s="2" t="inlineStr">
+      <c r="F60" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -2259,15 +2259,15 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
+          <t>1-2</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
           <t>0-1</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>0-1</t>
-        </is>
-      </c>
-      <c r="F61" s="3" t="inlineStr">
+      <c r="F61" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -2289,7 +2289,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -2297,7 +2297,7 @@
           <t>0-0</t>
         </is>
       </c>
-      <c r="F62" s="2" t="inlineStr">
+      <c r="F62" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -2319,7 +2319,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>1-1</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -2329,7 +2329,7 @@
       </c>
       <c r="F63" s="2" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>V</t>
         </is>
       </c>
     </row>
@@ -2357,7 +2357,7 @@
           <t>0-1</t>
         </is>
       </c>
-      <c r="F64" s="2" t="inlineStr">
+      <c r="F64" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -2387,7 +2387,7 @@
           <t>1-1</t>
         </is>
       </c>
-      <c r="F65" s="3" t="inlineStr">
+      <c r="F65" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>
@@ -2409,7 +2409,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>1-1</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -2419,7 +2419,7 @@
       </c>
       <c r="F66" s="2" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>V</t>
         </is>
       </c>
     </row>
@@ -2439,7 +2439,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>2-1</t>
+          <t>2-2</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -2447,7 +2447,7 @@
           <t>0-2</t>
         </is>
       </c>
-      <c r="F67" s="2" t="inlineStr">
+      <c r="F67" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -2469,7 +2469,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>0-2</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -2477,7 +2477,7 @@
           <t>0-4</t>
         </is>
       </c>
-      <c r="F68" s="3" t="inlineStr">
+      <c r="F68" s="2" t="inlineStr">
         <is>
           <t>V</t>
         </is>

</xml_diff>